<commit_message>
Update normalization order, removed from points
</commit_message>
<xml_diff>
--- a/examples/points/output/results_current.xlsx
+++ b/examples/points/output/results_current.xlsx
@@ -475,13 +475,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>59.38546826174614</v>
+        <v>59.38546826174608</v>
       </c>
       <c r="D2" t="n">
-        <v>66.77325732111021</v>
+        <v>63.42541336441336</v>
       </c>
       <c r="E2" t="n">
-        <v>58.80544482155141</v>
+        <v>60.25269418342985</v>
       </c>
       <c r="F2" t="n">
         <v>64</v>
@@ -500,13 +500,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>63.6919816035002</v>
+        <v>63.69198160350019</v>
       </c>
       <c r="D3" t="n">
-        <v>61.8919265456765</v>
+        <v>59.34815366659485</v>
       </c>
       <c r="E3" t="n">
-        <v>60.05505844542681</v>
+        <v>60.69160993535012</v>
       </c>
       <c r="F3" t="n">
         <v>64</v>
@@ -525,13 +525,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>53.36976784286878</v>
+        <v>53.36976784286875</v>
       </c>
       <c r="D4" t="n">
-        <v>61.3980948251095</v>
+        <v>57.45725422290129</v>
       </c>
       <c r="E4" t="n">
-        <v>60.81685439607869</v>
+        <v>61.87721363059931</v>
       </c>
       <c r="F4" t="n">
         <v>53</v>
@@ -550,13 +550,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>43.66932331144531</v>
+        <v>43.66932331144529</v>
       </c>
       <c r="D5" t="n">
-        <v>42.13527123899487</v>
+        <v>43.74418318903318</v>
       </c>
       <c r="E5" t="n">
-        <v>37.89039941509437</v>
+        <v>37.46096718471431</v>
       </c>
       <c r="F5" t="n">
         <v>53</v>
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50.67296479585271</v>
+        <v>50.67296479585266</v>
       </c>
       <c r="D6" t="n">
-        <v>54.51907723855087</v>
+        <v>55.66959984459985</v>
       </c>
       <c r="E6" t="n">
-        <v>68.759971346207</v>
+        <v>68.51289622239032</v>
       </c>
       <c r="F6" t="n">
         <v>53</v>
@@ -600,13 +600,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>47.1044793249133</v>
+        <v>47.10447932491324</v>
       </c>
       <c r="D7" t="n">
-        <v>50.52444127796041</v>
+        <v>51.75171604506604</v>
       </c>
       <c r="E7" t="n">
-        <v>45.49177210669703</v>
+        <v>45.52189756927075</v>
       </c>
       <c r="F7" t="n">
         <v>51</v>
@@ -625,13 +625,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>47.24525048090218</v>
+        <v>47.24525048090215</v>
       </c>
       <c r="D8" t="n">
-        <v>31.05428571428566</v>
+        <v>30.87666666666667</v>
       </c>
       <c r="E8" t="n">
-        <v>26.83939240046442</v>
+        <v>26.66666142760384</v>
       </c>
       <c r="F8" t="n">
         <v>50</v>
@@ -650,13 +650,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>56.80115788763776</v>
+        <v>56.80115788763771</v>
       </c>
       <c r="D9" t="n">
-        <v>47.65943650793645</v>
+        <v>45.90104682539683</v>
       </c>
       <c r="E9" t="n">
-        <v>38.97043308170639</v>
+        <v>39.19771935066926</v>
       </c>
       <c r="F9" t="n">
         <v>48</v>
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>59.72067959874509</v>
+        <v>59.72067959874503</v>
       </c>
       <c r="D10" t="n">
-        <v>53.38999999999996</v>
+        <v>51.92871212121212</v>
       </c>
       <c r="E10" t="n">
-        <v>58.36558470785909</v>
+        <v>56.73449758777912</v>
       </c>
       <c r="F10" t="n">
         <v>47</v>
@@ -700,13 +700,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>44.37461711343465</v>
+        <v>44.37461711343462</v>
       </c>
       <c r="D11" t="n">
-        <v>41.91478571428567</v>
+        <v>42.53244761904762</v>
       </c>
       <c r="E11" t="n">
-        <v>46.27660139956841</v>
+        <v>46.07711529981829</v>
       </c>
       <c r="F11" t="n">
         <v>46</v>
@@ -728,10 +728,10 @@
         <v>62.20018442703472</v>
       </c>
       <c r="D12" t="n">
-        <v>64.22429233511579</v>
+        <v>64.40317460317461</v>
       </c>
       <c r="E12" t="n">
-        <v>65.31039838789394</v>
+        <v>62.74252417702127</v>
       </c>
       <c r="F12" t="n">
         <v>45</v>
@@ -750,13 +750,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>49.22267902323278</v>
+        <v>49.22267902323276</v>
       </c>
       <c r="D13" t="n">
-        <v>40.29791605616602</v>
+        <v>40.64806966570016</v>
       </c>
       <c r="E13" t="n">
-        <v>38.82330330901567</v>
+        <v>38.72367737969628</v>
       </c>
       <c r="F13" t="n">
         <v>45</v>
@@ -775,13 +775,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>42.68994763311179</v>
+        <v>42.68994763311176</v>
       </c>
       <c r="D14" t="n">
-        <v>34.32792490842488</v>
+        <v>35.14800589410589</v>
       </c>
       <c r="E14" t="n">
-        <v>35.19130658144942</v>
+        <v>35.52907568278507</v>
       </c>
       <c r="F14" t="n">
         <v>45</v>
@@ -800,13 +800,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>43.12052624080594</v>
+        <v>43.12052624080591</v>
       </c>
       <c r="D15" t="n">
-        <v>39.81242341430495</v>
+        <v>40.10497413622962</v>
       </c>
       <c r="E15" t="n">
-        <v>34.78123125278224</v>
+        <v>35.43243130294851</v>
       </c>
       <c r="F15" t="n">
         <v>45</v>
@@ -825,13 +825,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>47.86508298030193</v>
+        <v>47.86508298030187</v>
       </c>
       <c r="D16" t="n">
-        <v>46.32810434854995</v>
+        <v>47.71483398193947</v>
       </c>
       <c r="E16" t="n">
-        <v>41.36496475192151</v>
+        <v>42.12552176162218</v>
       </c>
       <c r="F16" t="n">
         <v>43</v>
@@ -850,13 +850,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>49.9536404090103</v>
+        <v>49.95364040901026</v>
       </c>
       <c r="D17" t="n">
-        <v>43.0208777713514</v>
+        <v>43.87390155603205</v>
       </c>
       <c r="E17" t="n">
-        <v>36.53363508383594</v>
+        <v>36.41333354999449</v>
       </c>
       <c r="F17" t="n">
         <v>43</v>
@@ -875,13 +875,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>45.83116723423689</v>
+        <v>45.83116723423684</v>
       </c>
       <c r="D18" t="n">
-        <v>39.18246367521363</v>
+        <v>41.09538427350614</v>
       </c>
       <c r="E18" t="n">
-        <v>37.09690184781339</v>
+        <v>36.07436538694189</v>
       </c>
       <c r="F18" t="n">
         <v>43</v>
@@ -900,13 +900,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>39.63566181249222</v>
+        <v>39.63566181249215</v>
       </c>
       <c r="D19" t="n">
-        <v>38.84184418359416</v>
+        <v>38.72298087135274</v>
       </c>
       <c r="E19" t="n">
-        <v>34.98708282829138</v>
+        <v>34.91253421869783</v>
       </c>
       <c r="F19" t="n">
         <v>43</v>
@@ -925,13 +925,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>51.35483969458016</v>
+        <v>51.35483969458014</v>
       </c>
       <c r="D20" t="n">
-        <v>45.30430952380947</v>
+        <v>46.58742424242424</v>
       </c>
       <c r="E20" t="n">
-        <v>45.2632088611202</v>
+        <v>45.23626496759873</v>
       </c>
       <c r="F20" t="n">
         <v>42</v>
@@ -950,13 +950,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>54.08719086103525</v>
+        <v>54.08719086103523</v>
       </c>
       <c r="D21" t="n">
-        <v>50.83510317460312</v>
+        <v>51.03830555555555</v>
       </c>
       <c r="E21" t="n">
-        <v>55.27671185779263</v>
+        <v>54.76773480323697</v>
       </c>
       <c r="F21" t="n">
         <v>41</v>
@@ -975,13 +975,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>51.51552152684295</v>
+        <v>51.51552152684292</v>
       </c>
       <c r="D22" t="n">
-        <v>32.71999999999995</v>
+        <v>32.1</v>
       </c>
       <c r="E22" t="n">
-        <v>26.85270603574276</v>
+        <v>26.67034111386788</v>
       </c>
       <c r="F22" t="n">
         <v>41</v>
@@ -1000,13 +1000,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>45.08676889038884</v>
+        <v>45.08676889038882</v>
       </c>
       <c r="D23" t="n">
-        <v>43.14775304447011</v>
+        <v>45.20079481629481</v>
       </c>
       <c r="E23" t="n">
-        <v>44.45689089747574</v>
+        <v>44.63199339840013</v>
       </c>
       <c r="F23" t="n">
         <v>40</v>
@@ -1025,13 +1025,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>53.19295950995601</v>
+        <v>53.19295950995599</v>
       </c>
       <c r="D24" t="n">
-        <v>53.20662520136415</v>
+        <v>52.3081033153838</v>
       </c>
       <c r="E24" t="n">
-        <v>46.48051514418172</v>
+        <v>47.3087020138349</v>
       </c>
       <c r="F24" t="n">
         <v>40</v>
@@ -1050,13 +1050,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>28.56065668773325</v>
+        <v>28.56065668773319</v>
       </c>
       <c r="D25" t="n">
-        <v>19.41433333333331</v>
+        <v>19.89884615384615</v>
       </c>
       <c r="E25" t="n">
-        <v>19.16727612100999</v>
+        <v>19.58765366104738</v>
       </c>
       <c r="F25" t="n">
         <v>39</v>
@@ -1075,13 +1075,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>44.03095240163164</v>
+        <v>44.03095240163163</v>
       </c>
       <c r="D26" t="n">
-        <v>35.72862499999997</v>
+        <v>37.1186934629813</v>
       </c>
       <c r="E26" t="n">
-        <v>35.96818973294926</v>
+        <v>35.43699957584237</v>
       </c>
       <c r="F26" t="n">
         <v>39</v>
@@ -1100,13 +1100,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>51.78241724062207</v>
+        <v>51.78241724062203</v>
       </c>
       <c r="D27" t="n">
-        <v>45.21425885225879</v>
+        <v>43.93132462556601</v>
       </c>
       <c r="E27" t="n">
-        <v>36.72921505365216</v>
+        <v>38.31355018842704</v>
       </c>
       <c r="F27" t="n">
         <v>39</v>
@@ -1125,13 +1125,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>37.33634202935478</v>
+        <v>37.33634202935477</v>
       </c>
       <c r="D28" t="n">
-        <v>28.98697389212093</v>
+        <v>30.50826761310019</v>
       </c>
       <c r="E28" t="n">
-        <v>32.4165793654</v>
+        <v>31.90309722331293</v>
       </c>
       <c r="F28" t="n">
         <v>39</v>
@@ -1150,13 +1150,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>43.74879953340768</v>
+        <v>43.74879953340764</v>
       </c>
       <c r="D29" t="n">
-        <v>43.03641409613773</v>
+        <v>46.37322763347763</v>
       </c>
       <c r="E29" t="n">
-        <v>44.14339525860529</v>
+        <v>44.14074131299333</v>
       </c>
       <c r="F29" t="n">
         <v>39</v>
@@ -1175,13 +1175,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>34.507000994881</v>
+        <v>34.50700099488098</v>
       </c>
       <c r="D30" t="n">
-        <v>38.27340490065487</v>
+        <v>38.2431510149065</v>
       </c>
       <c r="E30" t="n">
-        <v>38.84522440053741</v>
+        <v>38.95307571422422</v>
       </c>
       <c r="F30" t="n">
         <v>38</v>
@@ -1200,13 +1200,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>36.56774375770209</v>
+        <v>36.56774375770203</v>
       </c>
       <c r="D31" t="n">
-        <v>31.32719047619043</v>
+        <v>30.12239610963749</v>
       </c>
       <c r="E31" t="n">
-        <v>30.68756615027909</v>
+        <v>30.59084053192337</v>
       </c>
       <c r="F31" t="n">
         <v>38</v>
@@ -1225,13 +1225,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>40.75189509662887</v>
+        <v>40.75189509662886</v>
       </c>
       <c r="D32" t="n">
-        <v>39.40240022112387</v>
+        <v>40.81971062845201</v>
       </c>
       <c r="E32" t="n">
-        <v>43.31739070626571</v>
+        <v>43.38266779290538</v>
       </c>
       <c r="F32" t="n">
         <v>38</v>
@@ -1250,13 +1250,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>47.39087136223547</v>
+        <v>47.39087136223544</v>
       </c>
       <c r="D33" t="n">
-        <v>40.34214120236485</v>
+        <v>41.03232216894405</v>
       </c>
       <c r="E33" t="n">
-        <v>40.27494113558616</v>
+        <v>39.51705705973465</v>
       </c>
       <c r="F33" t="n">
         <v>38</v>
@@ -1275,13 +1275,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>57.2454071211743</v>
+        <v>57.24540712117425</v>
       </c>
       <c r="D34" t="n">
-        <v>47.85669047619042</v>
+        <v>47.87742424242424</v>
       </c>
       <c r="E34" t="n">
-        <v>44.97177303434763</v>
+        <v>45.32694953026886</v>
       </c>
       <c r="F34" t="n">
         <v>38</v>
@@ -1300,13 +1300,13 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>38.05800914098638</v>
+        <v>38.05800914098634</v>
       </c>
       <c r="D35" t="n">
-        <v>40.69817170548747</v>
+        <v>40.0884352364321</v>
       </c>
       <c r="E35" t="n">
-        <v>41.12879906230716</v>
+        <v>41.1523649344886</v>
       </c>
       <c r="F35" t="n">
         <v>38</v>
@@ -1325,13 +1325,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>42.81738032077938</v>
+        <v>42.81738032077934</v>
       </c>
       <c r="D36" t="n">
-        <v>38.1925833333333</v>
+        <v>40.36733333333333</v>
       </c>
       <c r="E36" t="n">
-        <v>63.81250605569181</v>
+        <v>62.77227396819354</v>
       </c>
       <c r="F36" t="n">
         <v>38</v>
@@ -1350,13 +1350,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>51.19536910459493</v>
+        <v>51.19536910459487</v>
       </c>
       <c r="D37" t="n">
-        <v>47.24007936507931</v>
+        <v>47.03697222222222</v>
       </c>
       <c r="E37" t="n">
-        <v>46.74612466568656</v>
+        <v>45.56088084069845</v>
       </c>
       <c r="F37" t="n">
         <v>37</v>
@@ -1375,13 +1375,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>45.08677593929536</v>
+        <v>45.08677593929534</v>
       </c>
       <c r="D38" t="n">
-        <v>40.2652150729387</v>
+        <v>42.3638373015873</v>
       </c>
       <c r="E38" t="n">
-        <v>43.66533703766702</v>
+        <v>43.56481506888056</v>
       </c>
       <c r="F38" t="n">
         <v>37</v>
@@ -1400,13 +1400,13 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>34.33197206143393</v>
+        <v>34.33197206143388</v>
       </c>
       <c r="D39" t="n">
-        <v>35.55185390632756</v>
+        <v>36.44645916340811</v>
       </c>
       <c r="E39" t="n">
-        <v>35.03962630355272</v>
+        <v>34.96244565475296</v>
       </c>
       <c r="F39" t="n">
         <v>37</v>
@@ -1425,13 +1425,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>39.37789017126224</v>
+        <v>39.37789017126222</v>
       </c>
       <c r="D40" t="n">
-        <v>35.33983363858361</v>
+        <v>35.84637057312606</v>
       </c>
       <c r="E40" t="n">
-        <v>36.4724269451658</v>
+        <v>36.73792775874397</v>
       </c>
       <c r="F40" t="n">
         <v>36</v>
@@ -1450,13 +1450,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>45.11835864975566</v>
+        <v>45.11835864975564</v>
       </c>
       <c r="D41" t="n">
-        <v>28.32091666666662</v>
+        <v>27.44611111111111</v>
       </c>
       <c r="E41" t="n">
-        <v>30.22021031658518</v>
+        <v>30.24958098028898</v>
       </c>
       <c r="F41" t="n">
         <v>36</v>
@@ -1475,13 +1475,13 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>46.50614530105639</v>
+        <v>46.50614530105637</v>
       </c>
       <c r="D42" t="n">
-        <v>39.27156258215465</v>
+        <v>39.25224261035899</v>
       </c>
       <c r="E42" t="n">
-        <v>30.50666686319319</v>
+        <v>30.53722917304214</v>
       </c>
       <c r="F42" t="n">
         <v>36</v>
@@ -1500,13 +1500,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>33.06313786902617</v>
+        <v>33.06313786902613</v>
       </c>
       <c r="D43" t="n">
-        <v>33.04391040005743</v>
+        <v>32.1181168007689</v>
       </c>
       <c r="E43" t="n">
-        <v>35.27632400444873</v>
+        <v>35.10447396840081</v>
       </c>
       <c r="F43" t="n">
         <v>36</v>
@@ -1525,13 +1525,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>35.80382087681971</v>
+        <v>35.80382087681969</v>
       </c>
       <c r="D44" t="n">
-        <v>37.31285317460313</v>
+        <v>36.88245738169876</v>
       </c>
       <c r="E44" t="n">
-        <v>36.9952257875885</v>
+        <v>36.61873101986084</v>
       </c>
       <c r="F44" t="n">
         <v>35</v>
@@ -1550,13 +1550,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>50.00085294265958</v>
+        <v>50.00085294265956</v>
       </c>
       <c r="D45" t="n">
-        <v>24.43999999999996</v>
+        <v>25.08</v>
       </c>
       <c r="E45" t="n">
-        <v>26.00639642381033</v>
+        <v>25.60721428446496</v>
       </c>
       <c r="F45" t="n">
         <v>35</v>
@@ -1575,13 +1575,13 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>41.22313375181864</v>
+        <v>41.22313375181856</v>
       </c>
       <c r="D46" t="n">
-        <v>39.27544627594624</v>
+        <v>40.76448450660637</v>
       </c>
       <c r="E46" t="n">
-        <v>41.35688767836307</v>
+        <v>40.04057215194112</v>
       </c>
       <c r="F46" t="n">
         <v>35</v>
@@ -1600,13 +1600,13 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>48.09825429714516</v>
+        <v>48.09825429714507</v>
       </c>
       <c r="D47" t="n">
-        <v>42.05984920634913</v>
+        <v>39.73905694879832</v>
       </c>
       <c r="E47" t="n">
-        <v>36.57139945574618</v>
+        <v>36.63421608075304</v>
       </c>
       <c r="F47" t="n">
         <v>35</v>
@@ -1625,13 +1625,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>37.57173688665708</v>
+        <v>37.57173688665701</v>
       </c>
       <c r="D48" t="n">
-        <v>39.36659069731435</v>
+        <v>39.83309432734119</v>
       </c>
       <c r="E48" t="n">
-        <v>35.08202332108933</v>
+        <v>34.94292479086641</v>
       </c>
       <c r="F48" t="n">
         <v>35</v>
@@ -1650,13 +1650,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>38.14808735177997</v>
+        <v>38.1480873517799</v>
       </c>
       <c r="D49" t="n">
-        <v>47.331215062715</v>
+        <v>46.33571928646066</v>
       </c>
       <c r="E49" t="n">
-        <v>45.75746261401997</v>
+        <v>44.2954035351647</v>
       </c>
       <c r="F49" t="n">
         <v>35</v>
@@ -1675,13 +1675,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>39.54513693291508</v>
+        <v>39.54513693291504</v>
       </c>
       <c r="D50" t="n">
-        <v>31.20726190476186</v>
+        <v>31.10505128205128</v>
       </c>
       <c r="E50" t="n">
-        <v>33.46603388496951</v>
+        <v>31.70095182696163</v>
       </c>
       <c r="F50" t="n">
         <v>34</v>
@@ -1700,13 +1700,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>43.18222784449683</v>
+        <v>43.18222784449676</v>
       </c>
       <c r="D51" t="n">
-        <v>41.37027380952376</v>
+        <v>43.95487032297768</v>
       </c>
       <c r="E51" t="n">
-        <v>41.62353906163244</v>
+        <v>41.37920352978762</v>
       </c>
       <c r="F51" t="n">
         <v>34</v>
@@ -1728,10 +1728,10 @@
         <v>37.05637333713083</v>
       </c>
       <c r="D52" t="n">
-        <v>41.82606244778608</v>
+        <v>41.87653888888889</v>
       </c>
       <c r="E52" t="n">
-        <v>42.40888408846534</v>
+        <v>41.89737467212291</v>
       </c>
       <c r="F52" t="n">
         <v>34</v>
@@ -1750,13 +1750,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>36.76792133831401</v>
+        <v>36.76792133831399</v>
       </c>
       <c r="D53" t="n">
-        <v>31.81432361352096</v>
+        <v>31.58208825545799</v>
       </c>
       <c r="E53" t="n">
-        <v>37.08380295054825</v>
+        <v>37.81283730561255</v>
       </c>
       <c r="F53" t="n">
         <v>34</v>
@@ -1775,13 +1775,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>42.19270506812331</v>
+        <v>42.19270506812328</v>
       </c>
       <c r="D54" t="n">
-        <v>45.94430708180704</v>
+        <v>45.66385930735931</v>
       </c>
       <c r="E54" t="n">
-        <v>43.89707285236367</v>
+        <v>43.59427479493151</v>
       </c>
       <c r="F54" t="n">
         <v>33</v>
@@ -1800,13 +1800,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>40.47430644426496</v>
+        <v>40.4743064442649</v>
       </c>
       <c r="D55" t="n">
-        <v>35.92316085226009</v>
+        <v>34.76639202667251</v>
       </c>
       <c r="E55" t="n">
-        <v>35.88555496907714</v>
+        <v>34.81592209588304</v>
       </c>
       <c r="F55" t="n">
         <v>33</v>
@@ -1825,13 +1825,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>34.44450351678351</v>
+        <v>34.44450351678348</v>
       </c>
       <c r="D56" t="n">
-        <v>38.31432907589484</v>
+        <v>38.86158609374472</v>
       </c>
       <c r="E56" t="n">
-        <v>36.98965294546584</v>
+        <v>36.99360591388765</v>
       </c>
       <c r="F56" t="n">
         <v>33</v>
@@ -1850,13 +1850,13 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>30.08125403875603</v>
+        <v>30.08125403875599</v>
       </c>
       <c r="D57" t="n">
-        <v>21.23274999999999</v>
+        <v>21.74134615384615</v>
       </c>
       <c r="E57" t="n">
-        <v>21.59771078785032</v>
+        <v>20.7292267443771</v>
       </c>
       <c r="F57" t="n">
         <v>33</v>
@@ -1875,13 +1875,13 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>39.52411058550744</v>
+        <v>39.52411058550741</v>
       </c>
       <c r="D58" t="n">
-        <v>28.83833333333328</v>
+        <v>29.4080829228243</v>
       </c>
       <c r="E58" t="n">
-        <v>28.58980368773445</v>
+        <v>27.4438969786364</v>
       </c>
       <c r="F58" t="n">
         <v>33</v>
@@ -1900,13 +1900,13 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>37.38048006812592</v>
+        <v>37.38048006812594</v>
       </c>
       <c r="D59" t="n">
-        <v>21.95999999999998</v>
+        <v>22.69</v>
       </c>
       <c r="E59" t="n">
-        <v>19.19639760564682</v>
+        <v>19.7158637623344</v>
       </c>
       <c r="F59" t="n">
         <v>33</v>
@@ -1928,10 +1928,10 @@
         <v>35.6197954752062</v>
       </c>
       <c r="D60" t="n">
-        <v>39.741465034965</v>
+        <v>39.93611990990041</v>
       </c>
       <c r="E60" t="n">
-        <v>42.3289344885571</v>
+        <v>42.51523861216723</v>
       </c>
       <c r="F60" t="n">
         <v>33</v>
@@ -1950,13 +1950,13 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>38.30904159532447</v>
+        <v>38.30904159532444</v>
       </c>
       <c r="D61" t="n">
-        <v>39.49077018449384</v>
+        <v>39.35854941392128</v>
       </c>
       <c r="E61" t="n">
-        <v>40.57280218549623</v>
+        <v>40.47180526282247</v>
       </c>
       <c r="F61" t="n">
         <v>32</v>
@@ -1975,13 +1975,13 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>37.2711581808212</v>
+        <v>37.27115818082118</v>
       </c>
       <c r="D62" t="n">
-        <v>38.64620726495723</v>
+        <v>38.13262404836542</v>
       </c>
       <c r="E62" t="n">
-        <v>36.78566879407909</v>
+        <v>36.75552190991058</v>
       </c>
       <c r="F62" t="n">
         <v>32</v>
@@ -2000,13 +2000,13 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>35.1263455590267</v>
+        <v>35.12634555902668</v>
       </c>
       <c r="D63" t="n">
-        <v>35.17567186614551</v>
+        <v>36.99438356381614</v>
       </c>
       <c r="E63" t="n">
-        <v>32.80796054346003</v>
+        <v>32.80695537842051</v>
       </c>
       <c r="F63" t="n">
         <v>32</v>
@@ -2025,13 +2025,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>34.34404855230776</v>
+        <v>34.34404855230773</v>
       </c>
       <c r="D64" t="n">
-        <v>35.21933961506326</v>
+        <v>35.79166708291709</v>
       </c>
       <c r="E64" t="n">
-        <v>34.79640633601212</v>
+        <v>34.72680557445837</v>
       </c>
       <c r="F64" t="n">
         <v>31</v>
@@ -2050,13 +2050,13 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>39.10275641838586</v>
+        <v>39.10275641838584</v>
       </c>
       <c r="D65" t="n">
-        <v>30.99795906971135</v>
+        <v>30.35972943927417</v>
       </c>
       <c r="E65" t="n">
-        <v>27.47130514977526</v>
+        <v>27.91304784432847</v>
       </c>
       <c r="F65" t="n">
         <v>31</v>
@@ -2075,13 +2075,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>36.56007534179875</v>
+        <v>36.56007534179871</v>
       </c>
       <c r="D66" t="n">
-        <v>38.97181838629206</v>
+        <v>39.88934063087426</v>
       </c>
       <c r="E66" t="n">
-        <v>40.74665155502776</v>
+        <v>40.87794929879905</v>
       </c>
       <c r="F66" t="n">
         <v>31</v>
@@ -2100,13 +2100,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>24.35320758500584</v>
+        <v>24.3532075850058</v>
       </c>
       <c r="D67" t="n">
-        <v>30.27937896825394</v>
+        <v>31.24591545806568</v>
       </c>
       <c r="E67" t="n">
-        <v>30.38658059091648</v>
+        <v>30.24108988689332</v>
       </c>
       <c r="F67" t="n">
         <v>31</v>
@@ -2125,13 +2125,13 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>32.8486124879419</v>
+        <v>32.84861248794187</v>
       </c>
       <c r="D68" t="n">
-        <v>29.6979326100599</v>
+        <v>28.80179826375035</v>
       </c>
       <c r="E68" t="n">
-        <v>26.04483665688252</v>
+        <v>25.93293202234682</v>
       </c>
       <c r="F68" t="n">
         <v>31</v>
@@ -2150,13 +2150,13 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>34.14845374712574</v>
+        <v>34.14845374712571</v>
       </c>
       <c r="D69" t="n">
-        <v>39.90255738705735</v>
+        <v>39.87805276593325</v>
       </c>
       <c r="E69" t="n">
-        <v>38.14193150772542</v>
+        <v>37.96560558673822</v>
       </c>
       <c r="F69" t="n">
         <v>31</v>
@@ -2175,13 +2175,13 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>32.85372984707369</v>
+        <v>32.85372984707366</v>
       </c>
       <c r="D70" t="n">
-        <v>38.51766456788823</v>
+        <v>39.69558497558184</v>
       </c>
       <c r="E70" t="n">
-        <v>42.01789841350871</v>
+        <v>41.98605844998993</v>
       </c>
       <c r="F70" t="n">
         <v>31</v>
@@ -2200,13 +2200,13 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>35.01082274224603</v>
+        <v>35.01082274224598</v>
       </c>
       <c r="D71" t="n">
-        <v>31.2572779304029</v>
+        <v>32.99547931162406</v>
       </c>
       <c r="E71" t="n">
-        <v>33.95877573312261</v>
+        <v>34.09851140112691</v>
       </c>
       <c r="F71" t="n">
         <v>31</v>
@@ -2225,13 +2225,13 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>31.22922579513555</v>
+        <v>31.2292257951355</v>
       </c>
       <c r="D72" t="n">
-        <v>26.4858452380952</v>
+        <v>25.684</v>
       </c>
       <c r="E72" t="n">
-        <v>30.40755609333446</v>
+        <v>30.05652771798558</v>
       </c>
       <c r="F72" t="n">
         <v>31</v>
@@ -2250,13 +2250,13 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>27.61939485389355</v>
+        <v>27.61939485389352</v>
       </c>
       <c r="D73" t="n">
-        <v>27.73104292929288</v>
+        <v>26.99733333333333</v>
       </c>
       <c r="E73" t="n">
-        <v>33.66455059687406</v>
+        <v>31.2934420243233</v>
       </c>
       <c r="F73" t="n">
         <v>30</v>
@@ -2275,13 +2275,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>36.74685694885115</v>
+        <v>36.74685694885111</v>
       </c>
       <c r="D74" t="n">
-        <v>38.27895238095233</v>
+        <v>39.11138095238096</v>
       </c>
       <c r="E74" t="n">
-        <v>45.13366412120068</v>
+        <v>44.46910603826556</v>
       </c>
       <c r="F74" t="n">
         <v>30</v>
@@ -2300,13 +2300,13 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>34.03050098009047</v>
+        <v>34.03050098009043</v>
       </c>
       <c r="D75" t="n">
-        <v>33.72352659475024</v>
+        <v>34.98066304531619</v>
       </c>
       <c r="E75" t="n">
-        <v>35.16700117453538</v>
+        <v>35.69262495947584</v>
       </c>
       <c r="F75" t="n">
         <v>30</v>
@@ -2325,13 +2325,13 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>35.35716696824272</v>
+        <v>35.35716696824267</v>
       </c>
       <c r="D76" t="n">
-        <v>38.96871017871013</v>
+        <v>37.19400103249241</v>
       </c>
       <c r="E76" t="n">
-        <v>35.18515421594135</v>
+        <v>35.65333421113625</v>
       </c>
       <c r="F76" t="n">
         <v>29</v>
@@ -2350,13 +2350,13 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>27.14104584205288</v>
+        <v>27.14104584205284</v>
       </c>
       <c r="D77" t="n">
-        <v>22.81836111111108</v>
+        <v>25.49063492063492</v>
       </c>
       <c r="E77" t="n">
-        <v>19.38482397088862</v>
+        <v>19.23280894162854</v>
       </c>
       <c r="F77" t="n">
         <v>29</v>
@@ -2375,13 +2375,13 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>40.36755989908804</v>
+        <v>40.36755989908796</v>
       </c>
       <c r="D78" t="n">
-        <v>38.94099389499385</v>
+        <v>41.75939386724387</v>
       </c>
       <c r="E78" t="n">
-        <v>36.89585855305029</v>
+        <v>35.34490403344216</v>
       </c>
       <c r="F78" t="n">
         <v>29</v>
@@ -2400,13 +2400,13 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>28.73863907136154</v>
+        <v>28.7386390713615</v>
       </c>
       <c r="D79" t="n">
-        <v>30.459100551019</v>
+        <v>29.70483424091683</v>
       </c>
       <c r="E79" t="n">
-        <v>27.06487411209848</v>
+        <v>27.38349184134797</v>
       </c>
       <c r="F79" t="n">
         <v>29</v>
@@ -2425,13 +2425,13 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>31.52506827875184</v>
+        <v>31.5250682787518</v>
       </c>
       <c r="D80" t="n">
-        <v>22.71999999999997</v>
+        <v>24.24</v>
       </c>
       <c r="E80" t="n">
-        <v>27.56819710392553</v>
+        <v>25.18140690961703</v>
       </c>
       <c r="F80" t="n">
         <v>29</v>
@@ -2450,13 +2450,13 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>27.60288358506942</v>
+        <v>27.60288358506939</v>
       </c>
       <c r="D81" t="n">
-        <v>23.29999999999998</v>
+        <v>22.37</v>
       </c>
       <c r="E81" t="n">
-        <v>19.38482397088862</v>
+        <v>19.23280894162854</v>
       </c>
       <c r="F81" t="n">
         <v>29</v>
@@ -2475,13 +2475,13 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>30.18576692930435</v>
+        <v>30.1857669293043</v>
       </c>
       <c r="D82" t="n">
-        <v>31.28585425685421</v>
+        <v>32.48652950402088</v>
       </c>
       <c r="E82" t="n">
-        <v>33.582910477068</v>
+        <v>31.86383605923418</v>
       </c>
       <c r="F82" t="n">
         <v>29</v>
@@ -2500,13 +2500,13 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>19.33370459147614</v>
+        <v>19.3337045914761</v>
       </c>
       <c r="D83" t="n">
-        <v>18.70016666666664</v>
+        <v>19.50884615384615</v>
       </c>
       <c r="E83" t="n">
-        <v>12.47081123068248</v>
+        <v>12.73313190196711</v>
       </c>
       <c r="F83" t="n">
         <v>28</v>
@@ -2525,13 +2525,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>39.85534742758966</v>
+        <v>39.85534742758964</v>
       </c>
       <c r="D84" t="n">
-        <v>22.87999999999997</v>
+        <v>24.03</v>
       </c>
       <c r="E84" t="n">
-        <v>25.71759497045265</v>
+        <v>25.46167547821971</v>
       </c>
       <c r="F84" t="n">
         <v>28</v>
@@ -2550,13 +2550,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>36.82774462650476</v>
+        <v>36.82774462650475</v>
       </c>
       <c r="D85" t="n">
-        <v>27.19211111111107</v>
+        <v>27.35833333333333</v>
       </c>
       <c r="E85" t="n">
-        <v>28.60264081062441</v>
+        <v>27.40854501803841</v>
       </c>
       <c r="F85" t="n">
         <v>28</v>
@@ -2575,13 +2575,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>32.63421508646908</v>
+        <v>32.63421508646906</v>
       </c>
       <c r="D86" t="n">
-        <v>41.5282756410256</v>
+        <v>41.18150915953964</v>
       </c>
       <c r="E86" t="n">
-        <v>39.9075801754629</v>
+        <v>39.54766342034106</v>
       </c>
       <c r="F86" t="n">
         <v>28</v>
@@ -2600,13 +2600,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>36.20286898125072</v>
+        <v>36.20286898125067</v>
       </c>
       <c r="D87" t="n">
-        <v>36.54148443223439</v>
+        <v>33.93638821841743</v>
       </c>
       <c r="E87" t="n">
-        <v>36.06773842857952</v>
+        <v>36.06594382726142</v>
       </c>
       <c r="F87" t="n">
         <v>28</v>
@@ -2625,13 +2625,13 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>43.81649605606231</v>
+        <v>43.81649605606221</v>
       </c>
       <c r="D88" t="n">
-        <v>45.03846031746027</v>
+        <v>45.32141269841269</v>
       </c>
       <c r="E88" t="n">
-        <v>45.28666439678435</v>
+        <v>45.25927003249642</v>
       </c>
       <c r="F88" t="n">
         <v>28</v>
@@ -2650,13 +2650,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>33.35085225249448</v>
+        <v>33.35085225249447</v>
       </c>
       <c r="D89" t="n">
-        <v>30.54287619352323</v>
+        <v>30.13829916488174</v>
       </c>
       <c r="E89" t="n">
-        <v>29.78730545641319</v>
+        <v>30.52560080784748</v>
       </c>
       <c r="F89" t="n">
         <v>27</v>
@@ -2675,13 +2675,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>30.69755704308934</v>
+        <v>30.69755704308931</v>
       </c>
       <c r="D90" t="n">
-        <v>36.00406078278442</v>
+        <v>35.84513461466825</v>
       </c>
       <c r="E90" t="n">
-        <v>34.4960833716444</v>
+        <v>34.35955301360703</v>
       </c>
       <c r="F90" t="n">
         <v>27</v>
@@ -2700,13 +2700,13 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>36.12961302917176</v>
+        <v>36.12961302917173</v>
       </c>
       <c r="D91" t="n">
-        <v>40.3957933338591</v>
+        <v>39.91971360509409</v>
       </c>
       <c r="E91" t="n">
-        <v>40.34616082734853</v>
+        <v>40.90947243026224</v>
       </c>
       <c r="F91" t="n">
         <v>27</v>
@@ -2725,13 +2725,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>28.93093777562849</v>
+        <v>28.93093777562846</v>
       </c>
       <c r="D92" t="n">
-        <v>32.2021053595527</v>
+        <v>32.36851364950839</v>
       </c>
       <c r="E92" t="n">
-        <v>37.99357601230513</v>
+        <v>37.25992487944452</v>
       </c>
       <c r="F92" t="n">
         <v>27</v>
@@ -2750,13 +2750,13 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>15.63816124042482</v>
+        <v>15.63816124042479</v>
       </c>
       <c r="D93" t="n">
-        <v>20.26999999999997</v>
+        <v>21.67</v>
       </c>
       <c r="E93" t="n">
-        <v>20.56104589894687</v>
+        <v>20.51330425265638</v>
       </c>
       <c r="F93" t="n">
         <v>27</v>
@@ -2775,13 +2775,13 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>35.49084719664999</v>
+        <v>35.49084719664994</v>
       </c>
       <c r="D94" t="n">
-        <v>39.53396886446883</v>
+        <v>39.31493640193327</v>
       </c>
       <c r="E94" t="n">
-        <v>42.57311035019693</v>
+        <v>41.52836956645702</v>
       </c>
       <c r="F94" t="n">
         <v>27</v>
@@ -2800,13 +2800,13 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>30.62534084538532</v>
+        <v>30.6253408453853</v>
       </c>
       <c r="D95" t="n">
-        <v>28.21410908636138</v>
+        <v>28.56523837567095</v>
       </c>
       <c r="E95" t="n">
-        <v>25.2395634880979</v>
+        <v>26.36171535565745</v>
       </c>
       <c r="F95" t="n">
         <v>27</v>
@@ -2825,13 +2825,13 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>27.79850272091472</v>
+        <v>27.79850272091466</v>
       </c>
       <c r="D96" t="n">
-        <v>19.04433333333331</v>
+        <v>19.85</v>
       </c>
       <c r="E96" t="n">
-        <v>18.97741455948137</v>
+        <v>19.16336015686847</v>
       </c>
       <c r="F96" t="n">
         <v>27</v>
@@ -2850,13 +2850,13 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>38.11582547637092</v>
+        <v>38.11582547637088</v>
       </c>
       <c r="D97" t="n">
-        <v>46.48163975758537</v>
+        <v>43.73840907628956</v>
       </c>
       <c r="E97" t="n">
-        <v>39.87594751217008</v>
+        <v>40.51248723428098</v>
       </c>
       <c r="F97" t="n">
         <v>27</v>
@@ -2875,13 +2875,13 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>39.32879093821063</v>
+        <v>39.3287909382106</v>
       </c>
       <c r="D98" t="n">
-        <v>34.01934414224117</v>
+        <v>32.75017983535506</v>
       </c>
       <c r="E98" t="n">
-        <v>34.90134224165574</v>
+        <v>34.15954484488492</v>
       </c>
       <c r="F98" t="n">
         <v>27</v>
@@ -2900,13 +2900,13 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>24.82971165125407</v>
+        <v>24.82971165125401</v>
       </c>
       <c r="D99" t="n">
-        <v>18.09516666666665</v>
+        <v>17.97384615384615</v>
       </c>
       <c r="E99" t="n">
-        <v>12.98350072100784</v>
+        <v>12.85178597175648</v>
       </c>
       <c r="F99" t="n">
         <v>27</v>
@@ -2925,13 +2925,13 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>41.04860408715697</v>
+        <v>41.04860408715695</v>
       </c>
       <c r="D100" t="n">
-        <v>35.6066085303585</v>
+        <v>36.24671492970631</v>
       </c>
       <c r="E100" t="n">
-        <v>40.23647702405019</v>
+        <v>40.19435303257193</v>
       </c>
       <c r="F100" t="n">
         <v>27</v>
@@ -2950,13 +2950,13 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>28.25809723096309</v>
+        <v>28.25809723096305</v>
       </c>
       <c r="D101" t="n">
-        <v>25.26999999999996</v>
+        <v>26.58</v>
       </c>
       <c r="E101" t="n">
-        <v>33.50403175772847</v>
+        <v>31.20992232049713</v>
       </c>
       <c r="F101" t="n">
         <v>27</v>

</xml_diff>

<commit_message>
Refactored, created .joblib models, update visualizer
</commit_message>
<xml_diff>
--- a/examples/points/output/results_current.xlsx
+++ b/examples/points/output/results_current.xlsx
@@ -478,10 +478,10 @@
         <v>59.38546826174608</v>
       </c>
       <c r="D2" t="n">
-        <v>63.42541336441336</v>
+        <v>64.06837878787879</v>
       </c>
       <c r="E2" t="n">
-        <v>60.25269418342985</v>
+        <v>59.84425295967663</v>
       </c>
       <c r="F2" t="n">
         <v>64</v>
@@ -503,10 +503,10 @@
         <v>63.69198160350019</v>
       </c>
       <c r="D3" t="n">
-        <v>59.34815366659485</v>
+        <v>61.55034666210982</v>
       </c>
       <c r="E3" t="n">
-        <v>60.69160993535012</v>
+        <v>60.56706990799329</v>
       </c>
       <c r="F3" t="n">
         <v>64</v>
@@ -528,10 +528,10 @@
         <v>53.36976784286875</v>
       </c>
       <c r="D4" t="n">
-        <v>57.45725422290129</v>
+        <v>58.24035486409016</v>
       </c>
       <c r="E4" t="n">
-        <v>61.87721363059931</v>
+        <v>61.53701077352506</v>
       </c>
       <c r="F4" t="n">
         <v>53</v>
@@ -553,10 +553,10 @@
         <v>43.66932331144529</v>
       </c>
       <c r="D5" t="n">
-        <v>43.74418318903318</v>
+        <v>41.71302372073232</v>
       </c>
       <c r="E5" t="n">
-        <v>37.46096718471431</v>
+        <v>38.00609930405464</v>
       </c>
       <c r="F5" t="n">
         <v>53</v>
@@ -578,10 +578,10 @@
         <v>50.67296479585266</v>
       </c>
       <c r="D6" t="n">
-        <v>55.66959984459985</v>
+        <v>54.01909845125633</v>
       </c>
       <c r="E6" t="n">
-        <v>68.51289622239032</v>
+        <v>68.75316575940086</v>
       </c>
       <c r="F6" t="n">
         <v>53</v>
@@ -603,10 +603,10 @@
         <v>47.10447932491324</v>
       </c>
       <c r="D7" t="n">
-        <v>51.75171604506604</v>
+        <v>49.46649350649349</v>
       </c>
       <c r="E7" t="n">
-        <v>45.52189756927075</v>
+        <v>45.72520340557201</v>
       </c>
       <c r="F7" t="n">
         <v>51</v>
@@ -628,10 +628,10 @@
         <v>47.24525048090215</v>
       </c>
       <c r="D8" t="n">
-        <v>30.87666666666667</v>
+        <v>29.55603896103896</v>
       </c>
       <c r="E8" t="n">
-        <v>26.66666142760384</v>
+        <v>25.86373750773323</v>
       </c>
       <c r="F8" t="n">
         <v>50</v>
@@ -653,10 +653,10 @@
         <v>56.80115788763771</v>
       </c>
       <c r="D9" t="n">
-        <v>45.90104682539683</v>
+        <v>47.45203277899626</v>
       </c>
       <c r="E9" t="n">
-        <v>39.19771935066926</v>
+        <v>39.04870530039328</v>
       </c>
       <c r="F9" t="n">
         <v>48</v>
@@ -678,10 +678,10 @@
         <v>59.72067959874503</v>
       </c>
       <c r="D10" t="n">
-        <v>51.92871212121212</v>
+        <v>53.76388888888889</v>
       </c>
       <c r="E10" t="n">
-        <v>56.73449758777912</v>
+        <v>58.32595885812119</v>
       </c>
       <c r="F10" t="n">
         <v>47</v>
@@ -703,10 +703,10 @@
         <v>44.37461711343462</v>
       </c>
       <c r="D11" t="n">
-        <v>42.53244761904762</v>
+        <v>42.25939640768588</v>
       </c>
       <c r="E11" t="n">
-        <v>46.07711529981829</v>
+        <v>46.98573247777817</v>
       </c>
       <c r="F11" t="n">
         <v>46</v>
@@ -728,10 +728,10 @@
         <v>62.20018442703472</v>
       </c>
       <c r="D12" t="n">
-        <v>64.40317460317461</v>
+        <v>64.98061952861954</v>
       </c>
       <c r="E12" t="n">
-        <v>62.74252417702127</v>
+        <v>64.58291650277094</v>
       </c>
       <c r="F12" t="n">
         <v>45</v>
@@ -753,10 +753,10 @@
         <v>49.22267902323276</v>
       </c>
       <c r="D13" t="n">
-        <v>40.64806966570016</v>
+        <v>41.39887496816908</v>
       </c>
       <c r="E13" t="n">
-        <v>38.72367737969628</v>
+        <v>39.16014939746171</v>
       </c>
       <c r="F13" t="n">
         <v>45</v>
@@ -778,10 +778,10 @@
         <v>42.68994763311176</v>
       </c>
       <c r="D14" t="n">
-        <v>35.14800589410589</v>
+        <v>34.13571350725297</v>
       </c>
       <c r="E14" t="n">
-        <v>35.52907568278507</v>
+        <v>37.15661381471787</v>
       </c>
       <c r="F14" t="n">
         <v>45</v>
@@ -803,10 +803,10 @@
         <v>43.12052624080591</v>
       </c>
       <c r="D15" t="n">
-        <v>40.10497413622962</v>
+        <v>40.73956072685484</v>
       </c>
       <c r="E15" t="n">
-        <v>35.43243130294851</v>
+        <v>35.7236196909588</v>
       </c>
       <c r="F15" t="n">
         <v>45</v>
@@ -828,10 +828,10 @@
         <v>47.86508298030187</v>
       </c>
       <c r="D16" t="n">
-        <v>47.71483398193947</v>
+        <v>47.28067523310678</v>
       </c>
       <c r="E16" t="n">
-        <v>42.12552176162218</v>
+        <v>41.23735422798637</v>
       </c>
       <c r="F16" t="n">
         <v>43</v>
@@ -853,10 +853,10 @@
         <v>49.95364040901026</v>
       </c>
       <c r="D17" t="n">
-        <v>43.87390155603205</v>
+        <v>41.33839177848755</v>
       </c>
       <c r="E17" t="n">
-        <v>36.41333354999449</v>
+        <v>36.35349356871298</v>
       </c>
       <c r="F17" t="n">
         <v>43</v>
@@ -878,10 +878,10 @@
         <v>45.83116723423684</v>
       </c>
       <c r="D18" t="n">
-        <v>41.09538427350614</v>
+        <v>39.68661306340719</v>
       </c>
       <c r="E18" t="n">
-        <v>36.07436538694189</v>
+        <v>37.88711381948541</v>
       </c>
       <c r="F18" t="n">
         <v>43</v>
@@ -903,10 +903,10 @@
         <v>39.63566181249215</v>
       </c>
       <c r="D19" t="n">
-        <v>38.72298087135274</v>
+        <v>39.35868882098294</v>
       </c>
       <c r="E19" t="n">
-        <v>34.91253421869783</v>
+        <v>35.29663048595945</v>
       </c>
       <c r="F19" t="n">
         <v>43</v>
@@ -928,10 +928,10 @@
         <v>51.35483969458014</v>
       </c>
       <c r="D20" t="n">
-        <v>46.58742424242424</v>
+        <v>46.08209451659452</v>
       </c>
       <c r="E20" t="n">
-        <v>45.23626496759873</v>
+        <v>45.58172785492273</v>
       </c>
       <c r="F20" t="n">
         <v>42</v>
@@ -953,10 +953,10 @@
         <v>54.08719086103523</v>
       </c>
       <c r="D21" t="n">
-        <v>51.03830555555555</v>
+        <v>50.42520634920636</v>
       </c>
       <c r="E21" t="n">
-        <v>54.76773480323697</v>
+        <v>55.03270735311763</v>
       </c>
       <c r="F21" t="n">
         <v>41</v>
@@ -978,10 +978,10 @@
         <v>51.51552152684292</v>
       </c>
       <c r="D22" t="n">
-        <v>32.1</v>
+        <v>30.64818181818182</v>
       </c>
       <c r="E22" t="n">
-        <v>26.67034111386788</v>
+        <v>25.88491838617546</v>
       </c>
       <c r="F22" t="n">
         <v>41</v>
@@ -1003,10 +1003,10 @@
         <v>45.08676889038882</v>
       </c>
       <c r="D23" t="n">
-        <v>45.20079481629481</v>
+        <v>44.41039410231347</v>
       </c>
       <c r="E23" t="n">
-        <v>44.63199339840013</v>
+        <v>44.4056152327994</v>
       </c>
       <c r="F23" t="n">
         <v>40</v>
@@ -1028,10 +1028,10 @@
         <v>53.19295950995599</v>
       </c>
       <c r="D24" t="n">
-        <v>52.3081033153838</v>
+        <v>50.70654473641049</v>
       </c>
       <c r="E24" t="n">
-        <v>47.3087020138349</v>
+        <v>47.23604523523893</v>
       </c>
       <c r="F24" t="n">
         <v>40</v>
@@ -1053,10 +1053,10 @@
         <v>28.56065668773319</v>
       </c>
       <c r="D25" t="n">
-        <v>19.89884615384615</v>
+        <v>18.54020833333333</v>
       </c>
       <c r="E25" t="n">
-        <v>19.58765366104738</v>
+        <v>19.77458900418357</v>
       </c>
       <c r="F25" t="n">
         <v>39</v>
@@ -1078,10 +1078,10 @@
         <v>44.03095240163163</v>
       </c>
       <c r="D26" t="n">
-        <v>37.1186934629813</v>
+        <v>36.32809592385598</v>
       </c>
       <c r="E26" t="n">
-        <v>35.43699957584237</v>
+        <v>35.55047231162576</v>
       </c>
       <c r="F26" t="n">
         <v>39</v>
@@ -1103,10 +1103,10 @@
         <v>51.78241724062203</v>
       </c>
       <c r="D27" t="n">
-        <v>43.93132462556601</v>
+        <v>44.56900198412699</v>
       </c>
       <c r="E27" t="n">
-        <v>38.31355018842704</v>
+        <v>38.46758346512251</v>
       </c>
       <c r="F27" t="n">
         <v>39</v>
@@ -1128,10 +1128,10 @@
         <v>37.33634202935477</v>
       </c>
       <c r="D28" t="n">
-        <v>30.50826761310019</v>
+        <v>30.91148763526336</v>
       </c>
       <c r="E28" t="n">
-        <v>31.90309722331293</v>
+        <v>32.09861385459853</v>
       </c>
       <c r="F28" t="n">
         <v>39</v>
@@ -1153,10 +1153,10 @@
         <v>43.74879953340764</v>
       </c>
       <c r="D29" t="n">
-        <v>46.37322763347763</v>
+        <v>44.93090091706539</v>
       </c>
       <c r="E29" t="n">
-        <v>44.14074131299333</v>
+        <v>44.06784808150861</v>
       </c>
       <c r="F29" t="n">
         <v>39</v>
@@ -1178,10 +1178,10 @@
         <v>34.50700099488098</v>
       </c>
       <c r="D30" t="n">
-        <v>38.2431510149065</v>
+        <v>38.01199543103955</v>
       </c>
       <c r="E30" t="n">
-        <v>38.95307571422422</v>
+        <v>39.11935068379585</v>
       </c>
       <c r="F30" t="n">
         <v>38</v>
@@ -1203,10 +1203,10 @@
         <v>36.56774375770203</v>
       </c>
       <c r="D31" t="n">
-        <v>30.12239610963749</v>
+        <v>29.77734848484849</v>
       </c>
       <c r="E31" t="n">
-        <v>30.59084053192337</v>
+        <v>29.71556712313844</v>
       </c>
       <c r="F31" t="n">
         <v>38</v>
@@ -1228,10 +1228,10 @@
         <v>40.75189509662886</v>
       </c>
       <c r="D32" t="n">
-        <v>40.81971062845201</v>
+        <v>39.56308706425153</v>
       </c>
       <c r="E32" t="n">
-        <v>43.38266779290538</v>
+        <v>43.21792299167637</v>
       </c>
       <c r="F32" t="n">
         <v>38</v>
@@ -1253,10 +1253,10 @@
         <v>47.39087136223544</v>
       </c>
       <c r="D33" t="n">
-        <v>41.03232216894405</v>
+        <v>39.99863447109306</v>
       </c>
       <c r="E33" t="n">
-        <v>39.51705705973465</v>
+        <v>41.34895419052308</v>
       </c>
       <c r="F33" t="n">
         <v>38</v>
@@ -1278,10 +1278,10 @@
         <v>57.24540712117425</v>
       </c>
       <c r="D34" t="n">
-        <v>47.87742424242424</v>
+        <v>46.65592784992786</v>
       </c>
       <c r="E34" t="n">
-        <v>45.32694953026886</v>
+        <v>45.37695098806102</v>
       </c>
       <c r="F34" t="n">
         <v>38</v>
@@ -1303,10 +1303,10 @@
         <v>38.05800914098634</v>
       </c>
       <c r="D35" t="n">
-        <v>40.0884352364321</v>
+        <v>40.26136259471193</v>
       </c>
       <c r="E35" t="n">
-        <v>41.1523649344886</v>
+        <v>41.62545628710904</v>
       </c>
       <c r="F35" t="n">
         <v>38</v>
@@ -1328,10 +1328,10 @@
         <v>42.81738032077934</v>
       </c>
       <c r="D36" t="n">
-        <v>40.36733333333333</v>
+        <v>39.29325613275613</v>
       </c>
       <c r="E36" t="n">
-        <v>62.77227396819354</v>
+        <v>64.87083386795138</v>
       </c>
       <c r="F36" t="n">
         <v>38</v>
@@ -1353,10 +1353,10 @@
         <v>51.19536910459487</v>
       </c>
       <c r="D37" t="n">
-        <v>47.03697222222222</v>
+        <v>46.47389682539684</v>
       </c>
       <c r="E37" t="n">
-        <v>45.56088084069845</v>
+        <v>46.22458593673435</v>
       </c>
       <c r="F37" t="n">
         <v>37</v>
@@ -1378,10 +1378,10 @@
         <v>45.08677593929534</v>
       </c>
       <c r="D38" t="n">
-        <v>42.3638373015873</v>
+        <v>40.67337256633116</v>
       </c>
       <c r="E38" t="n">
-        <v>43.56481506888056</v>
+        <v>43.9632128497305</v>
       </c>
       <c r="F38" t="n">
         <v>37</v>
@@ -1403,10 +1403,10 @@
         <v>34.33197206143388</v>
       </c>
       <c r="D39" t="n">
-        <v>36.44645916340811</v>
+        <v>36.30057134968612</v>
       </c>
       <c r="E39" t="n">
-        <v>34.96244565475296</v>
+        <v>35.46121275041813</v>
       </c>
       <c r="F39" t="n">
         <v>37</v>
@@ -1428,10 +1428,10 @@
         <v>39.37789017126222</v>
       </c>
       <c r="D40" t="n">
-        <v>35.84637057312606</v>
+        <v>36.19551700831847</v>
       </c>
       <c r="E40" t="n">
-        <v>36.73792775874397</v>
+        <v>36.89602232365407</v>
       </c>
       <c r="F40" t="n">
         <v>36</v>
@@ -1453,10 +1453,10 @@
         <v>45.11835864975564</v>
       </c>
       <c r="D41" t="n">
-        <v>27.44611111111111</v>
+        <v>27.22242857142857</v>
       </c>
       <c r="E41" t="n">
-        <v>30.24958098028898</v>
+        <v>29.3002740034066</v>
       </c>
       <c r="F41" t="n">
         <v>36</v>
@@ -1478,10 +1478,10 @@
         <v>46.50614530105637</v>
       </c>
       <c r="D42" t="n">
-        <v>39.25224261035899</v>
+        <v>39.0263298116348</v>
       </c>
       <c r="E42" t="n">
-        <v>30.53722917304214</v>
+        <v>30.08450485704697</v>
       </c>
       <c r="F42" t="n">
         <v>36</v>
@@ -1503,10 +1503,10 @@
         <v>33.06313786902613</v>
       </c>
       <c r="D43" t="n">
-        <v>32.1181168007689</v>
+        <v>34.40411287259912</v>
       </c>
       <c r="E43" t="n">
-        <v>35.10447396840081</v>
+        <v>34.99802117805959</v>
       </c>
       <c r="F43" t="n">
         <v>36</v>
@@ -1528,10 +1528,10 @@
         <v>35.80382087681969</v>
       </c>
       <c r="D44" t="n">
-        <v>36.88245738169876</v>
+        <v>36.96029897155983</v>
       </c>
       <c r="E44" t="n">
-        <v>36.61873101986084</v>
+        <v>36.75841861936163</v>
       </c>
       <c r="F44" t="n">
         <v>35</v>
@@ -1553,10 +1553,10 @@
         <v>50.00085294265956</v>
       </c>
       <c r="D45" t="n">
-        <v>25.08</v>
+        <v>25.526</v>
       </c>
       <c r="E45" t="n">
-        <v>25.60721428446496</v>
+        <v>25.38782237204057</v>
       </c>
       <c r="F45" t="n">
         <v>35</v>
@@ -1578,10 +1578,10 @@
         <v>41.22313375181856</v>
       </c>
       <c r="D46" t="n">
-        <v>40.76448450660637</v>
+        <v>39.47559984855187</v>
       </c>
       <c r="E46" t="n">
-        <v>40.04057215194112</v>
+        <v>41.70152784713847</v>
       </c>
       <c r="F46" t="n">
         <v>35</v>
@@ -1603,10 +1603,10 @@
         <v>48.09825429714507</v>
       </c>
       <c r="D47" t="n">
-        <v>39.73905694879832</v>
+        <v>39.9173722943723</v>
       </c>
       <c r="E47" t="n">
-        <v>36.63421608075304</v>
+        <v>37.65117938634997</v>
       </c>
       <c r="F47" t="n">
         <v>35</v>
@@ -1628,10 +1628,10 @@
         <v>37.57173688665701</v>
       </c>
       <c r="D48" t="n">
-        <v>39.83309432734119</v>
+        <v>39.96568677411677</v>
       </c>
       <c r="E48" t="n">
-        <v>34.94292479086641</v>
+        <v>35.46250763578717</v>
       </c>
       <c r="F48" t="n">
         <v>35</v>
@@ -1653,10 +1653,10 @@
         <v>38.1480873517799</v>
       </c>
       <c r="D49" t="n">
-        <v>46.33571928646066</v>
+        <v>46.27435209235209</v>
       </c>
       <c r="E49" t="n">
-        <v>44.2954035351647</v>
+        <v>44.77464981582826</v>
       </c>
       <c r="F49" t="n">
         <v>35</v>
@@ -1678,10 +1678,10 @@
         <v>39.54513693291504</v>
       </c>
       <c r="D50" t="n">
-        <v>31.10505128205128</v>
+        <v>31.05797619047619</v>
       </c>
       <c r="E50" t="n">
-        <v>31.70095182696163</v>
+        <v>30.78389687669682</v>
       </c>
       <c r="F50" t="n">
         <v>34</v>
@@ -1703,10 +1703,10 @@
         <v>43.18222784449676</v>
       </c>
       <c r="D51" t="n">
-        <v>43.95487032297768</v>
+        <v>43.18885945590358</v>
       </c>
       <c r="E51" t="n">
-        <v>41.37920352978762</v>
+        <v>41.50542879081895</v>
       </c>
       <c r="F51" t="n">
         <v>34</v>
@@ -1728,10 +1728,10 @@
         <v>37.05637333713083</v>
       </c>
       <c r="D52" t="n">
-        <v>41.87653888888889</v>
+        <v>40.31622808581167</v>
       </c>
       <c r="E52" t="n">
-        <v>41.89737467212291</v>
+        <v>42.0651103980024</v>
       </c>
       <c r="F52" t="n">
         <v>34</v>
@@ -1753,10 +1753,10 @@
         <v>36.76792133831399</v>
       </c>
       <c r="D53" t="n">
-        <v>31.58208825545799</v>
+        <v>31.7990858546768</v>
       </c>
       <c r="E53" t="n">
-        <v>37.81283730561255</v>
+        <v>37.65420360422194</v>
       </c>
       <c r="F53" t="n">
         <v>34</v>
@@ -1778,10 +1778,10 @@
         <v>42.19270506812328</v>
       </c>
       <c r="D54" t="n">
-        <v>45.66385930735931</v>
+        <v>46.06554094516595</v>
       </c>
       <c r="E54" t="n">
-        <v>43.59427479493151</v>
+        <v>43.71240253861264</v>
       </c>
       <c r="F54" t="n">
         <v>33</v>
@@ -1803,10 +1803,10 @@
         <v>40.4743064442649</v>
       </c>
       <c r="D55" t="n">
-        <v>34.76639202667251</v>
+        <v>36.7284340148791</v>
       </c>
       <c r="E55" t="n">
-        <v>34.81592209588304</v>
+        <v>35.48918322640261</v>
       </c>
       <c r="F55" t="n">
         <v>33</v>
@@ -1828,10 +1828,10 @@
         <v>34.44450351678348</v>
       </c>
       <c r="D56" t="n">
-        <v>38.86158609374472</v>
+        <v>38.16477774120904</v>
       </c>
       <c r="E56" t="n">
-        <v>36.99360591388765</v>
+        <v>36.52287391969227</v>
       </c>
       <c r="F56" t="n">
         <v>33</v>
@@ -1853,10 +1853,10 @@
         <v>30.08125403875599</v>
       </c>
       <c r="D57" t="n">
-        <v>21.74134615384615</v>
+        <v>20.20264705882353</v>
       </c>
       <c r="E57" t="n">
-        <v>20.7292267443771</v>
+        <v>20.83838524121962</v>
       </c>
       <c r="F57" t="n">
         <v>33</v>
@@ -1878,10 +1878,10 @@
         <v>39.52411058550741</v>
       </c>
       <c r="D58" t="n">
-        <v>29.4080829228243</v>
+        <v>28.88286324786325</v>
       </c>
       <c r="E58" t="n">
-        <v>27.4438969786364</v>
+        <v>26.5040406612774</v>
       </c>
       <c r="F58" t="n">
         <v>33</v>
@@ -1903,10 +1903,10 @@
         <v>37.38048006812594</v>
       </c>
       <c r="D59" t="n">
-        <v>22.69</v>
+        <v>24.06</v>
       </c>
       <c r="E59" t="n">
-        <v>19.7158637623344</v>
+        <v>20.15897489129349</v>
       </c>
       <c r="F59" t="n">
         <v>33</v>
@@ -1928,10 +1928,10 @@
         <v>35.6197954752062</v>
       </c>
       <c r="D60" t="n">
-        <v>39.93611990990041</v>
+        <v>38.84962166445526</v>
       </c>
       <c r="E60" t="n">
-        <v>42.51523861216723</v>
+        <v>43.04580762963927</v>
       </c>
       <c r="F60" t="n">
         <v>33</v>
@@ -1953,10 +1953,10 @@
         <v>38.30904159532444</v>
       </c>
       <c r="D61" t="n">
-        <v>39.35854941392128</v>
+        <v>39.19421817467018</v>
       </c>
       <c r="E61" t="n">
-        <v>40.47180526282247</v>
+        <v>40.98454890875121</v>
       </c>
       <c r="F61" t="n">
         <v>32</v>
@@ -1978,10 +1978,10 @@
         <v>37.27115818082118</v>
       </c>
       <c r="D62" t="n">
-        <v>38.13262404836542</v>
+        <v>37.7986948257057</v>
       </c>
       <c r="E62" t="n">
-        <v>36.75552190991058</v>
+        <v>36.38801507393579</v>
       </c>
       <c r="F62" t="n">
         <v>32</v>
@@ -2003,10 +2003,10 @@
         <v>35.12634555902668</v>
       </c>
       <c r="D63" t="n">
-        <v>36.99438356381614</v>
+        <v>35.90832315921653</v>
       </c>
       <c r="E63" t="n">
-        <v>32.80695537842051</v>
+        <v>33.79631638272424</v>
       </c>
       <c r="F63" t="n">
         <v>32</v>
@@ -2028,10 +2028,10 @@
         <v>34.34404855230773</v>
       </c>
       <c r="D64" t="n">
-        <v>35.79166708291709</v>
+        <v>36.71849089244948</v>
       </c>
       <c r="E64" t="n">
-        <v>34.72680557445837</v>
+        <v>35.97863483894802</v>
       </c>
       <c r="F64" t="n">
         <v>31</v>
@@ -2053,10 +2053,10 @@
         <v>39.10275641838584</v>
       </c>
       <c r="D65" t="n">
-        <v>30.35972943927417</v>
+        <v>29.63039983188628</v>
       </c>
       <c r="E65" t="n">
-        <v>27.91304784432847</v>
+        <v>27.35353213510064</v>
       </c>
       <c r="F65" t="n">
         <v>31</v>
@@ -2078,10 +2078,10 @@
         <v>36.56007534179871</v>
       </c>
       <c r="D66" t="n">
-        <v>39.88934063087426</v>
+        <v>39.31295633788632</v>
       </c>
       <c r="E66" t="n">
-        <v>40.87794929879905</v>
+        <v>40.62151599216508</v>
       </c>
       <c r="F66" t="n">
         <v>31</v>
@@ -2103,10 +2103,10 @@
         <v>24.3532075850058</v>
       </c>
       <c r="D67" t="n">
-        <v>31.24591545806568</v>
+        <v>31.00887607256341</v>
       </c>
       <c r="E67" t="n">
-        <v>30.24108988689332</v>
+        <v>29.79003027566268</v>
       </c>
       <c r="F67" t="n">
         <v>31</v>
@@ -2128,10 +2128,10 @@
         <v>32.84861248794187</v>
       </c>
       <c r="D68" t="n">
-        <v>28.80179826375035</v>
+        <v>31.20528256172953</v>
       </c>
       <c r="E68" t="n">
-        <v>25.93293202234682</v>
+        <v>26.24899838623301</v>
       </c>
       <c r="F68" t="n">
         <v>31</v>
@@ -2153,10 +2153,10 @@
         <v>34.14845374712571</v>
       </c>
       <c r="D69" t="n">
-        <v>39.87805276593325</v>
+        <v>39.45121263050675</v>
       </c>
       <c r="E69" t="n">
-        <v>37.96560558673822</v>
+        <v>38.97630305545511</v>
       </c>
       <c r="F69" t="n">
         <v>31</v>
@@ -2178,10 +2178,10 @@
         <v>32.85372984707366</v>
       </c>
       <c r="D70" t="n">
-        <v>39.69558497558184</v>
+        <v>39.26548137206984</v>
       </c>
       <c r="E70" t="n">
-        <v>41.98605844998993</v>
+        <v>42.39086727033409</v>
       </c>
       <c r="F70" t="n">
         <v>31</v>
@@ -2203,10 +2203,10 @@
         <v>35.01082274224598</v>
       </c>
       <c r="D71" t="n">
-        <v>32.99547931162406</v>
+        <v>29.89458390255816</v>
       </c>
       <c r="E71" t="n">
-        <v>34.09851140112691</v>
+        <v>34.41341612400202</v>
       </c>
       <c r="F71" t="n">
         <v>31</v>
@@ -2228,10 +2228,10 @@
         <v>31.2292257951355</v>
       </c>
       <c r="D72" t="n">
-        <v>25.684</v>
+        <v>25.47380769230769</v>
       </c>
       <c r="E72" t="n">
-        <v>30.05652771798558</v>
+        <v>29.42118002750522</v>
       </c>
       <c r="F72" t="n">
         <v>31</v>
@@ -2253,10 +2253,10 @@
         <v>27.61939485389352</v>
       </c>
       <c r="D73" t="n">
-        <v>26.99733333333333</v>
+        <v>26.25833333333333</v>
       </c>
       <c r="E73" t="n">
-        <v>31.2934420243233</v>
+        <v>30.21629842730912</v>
       </c>
       <c r="F73" t="n">
         <v>30</v>
@@ -2278,10 +2278,10 @@
         <v>36.74685694885111</v>
       </c>
       <c r="D74" t="n">
-        <v>39.11138095238096</v>
+        <v>38.97570015948963</v>
       </c>
       <c r="E74" t="n">
-        <v>44.46910603826556</v>
+        <v>44.23134812690625</v>
       </c>
       <c r="F74" t="n">
         <v>30</v>
@@ -2303,10 +2303,10 @@
         <v>34.03050098009043</v>
       </c>
       <c r="D75" t="n">
-        <v>34.98066304531619</v>
+        <v>34.91162219724719</v>
       </c>
       <c r="E75" t="n">
-        <v>35.69262495947584</v>
+        <v>35.32013619512061</v>
       </c>
       <c r="F75" t="n">
         <v>30</v>
@@ -2328,10 +2328,10 @@
         <v>35.35716696824267</v>
       </c>
       <c r="D76" t="n">
-        <v>37.19400103249241</v>
+        <v>37.42913620377207</v>
       </c>
       <c r="E76" t="n">
-        <v>35.65333421113625</v>
+        <v>35.22996684428198</v>
       </c>
       <c r="F76" t="n">
         <v>29</v>
@@ -2353,10 +2353,10 @@
         <v>27.14104584205284</v>
       </c>
       <c r="D77" t="n">
-        <v>25.49063492063492</v>
+        <v>24.31270833333333</v>
       </c>
       <c r="E77" t="n">
-        <v>19.23280894162854</v>
+        <v>19.63878591899063</v>
       </c>
       <c r="F77" t="n">
         <v>29</v>
@@ -2378,10 +2378,10 @@
         <v>40.36755989908796</v>
       </c>
       <c r="D78" t="n">
-        <v>41.75939386724387</v>
+        <v>42.1227766955267</v>
       </c>
       <c r="E78" t="n">
-        <v>35.34490403344216</v>
+        <v>37.71781141935417</v>
       </c>
       <c r="F78" t="n">
         <v>29</v>
@@ -2403,10 +2403,10 @@
         <v>28.7386390713615</v>
       </c>
       <c r="D79" t="n">
-        <v>29.70483424091683</v>
+        <v>30.30672980842918</v>
       </c>
       <c r="E79" t="n">
-        <v>27.38349184134797</v>
+        <v>26.78975191519803</v>
       </c>
       <c r="F79" t="n">
         <v>29</v>
@@ -2428,10 +2428,10 @@
         <v>31.5250682787518</v>
       </c>
       <c r="D80" t="n">
-        <v>24.24</v>
+        <v>24.98666666666666</v>
       </c>
       <c r="E80" t="n">
-        <v>25.18140690961703</v>
+        <v>25.66056776742708</v>
       </c>
       <c r="F80" t="n">
         <v>29</v>
@@ -2453,10 +2453,10 @@
         <v>27.60288358506939</v>
       </c>
       <c r="D81" t="n">
-        <v>22.37</v>
+        <v>20.7225</v>
       </c>
       <c r="E81" t="n">
-        <v>19.23280894162854</v>
+        <v>19.63878591899063</v>
       </c>
       <c r="F81" t="n">
         <v>29</v>
@@ -2478,10 +2478,10 @@
         <v>30.1857669293043</v>
       </c>
       <c r="D82" t="n">
-        <v>32.48652950402088</v>
+        <v>32.36337512079424</v>
       </c>
       <c r="E82" t="n">
-        <v>31.86383605923418</v>
+        <v>31.00911997441438</v>
       </c>
       <c r="F82" t="n">
         <v>29</v>
@@ -2503,10 +2503,10 @@
         <v>19.3337045914761</v>
       </c>
       <c r="D83" t="n">
-        <v>19.50884615384615</v>
+        <v>18.22202205882353</v>
       </c>
       <c r="E83" t="n">
-        <v>12.73313190196711</v>
+        <v>12.98118182709617</v>
       </c>
       <c r="F83" t="n">
         <v>28</v>
@@ -2528,10 +2528,10 @@
         <v>39.85534742758964</v>
       </c>
       <c r="D84" t="n">
-        <v>24.03</v>
+        <v>23.766</v>
       </c>
       <c r="E84" t="n">
-        <v>25.46167547821971</v>
+        <v>25.21152844734768</v>
       </c>
       <c r="F84" t="n">
         <v>28</v>
@@ -2553,10 +2553,10 @@
         <v>36.82774462650475</v>
       </c>
       <c r="D85" t="n">
-        <v>27.35833333333333</v>
+        <v>26.72891375291375</v>
       </c>
       <c r="E85" t="n">
-        <v>27.40854501803841</v>
+        <v>26.19268616222485</v>
       </c>
       <c r="F85" t="n">
         <v>28</v>
@@ -2578,10 +2578,10 @@
         <v>32.63421508646906</v>
       </c>
       <c r="D86" t="n">
-        <v>41.18150915953964</v>
+        <v>39.67214475247834</v>
       </c>
       <c r="E86" t="n">
-        <v>39.54766342034106</v>
+        <v>39.67998367920553</v>
       </c>
       <c r="F86" t="n">
         <v>28</v>
@@ -2603,10 +2603,10 @@
         <v>36.20286898125067</v>
       </c>
       <c r="D87" t="n">
-        <v>33.93638821841743</v>
+        <v>35.2892022170072</v>
       </c>
       <c r="E87" t="n">
-        <v>36.06594382726142</v>
+        <v>36.08953270209928</v>
       </c>
       <c r="F87" t="n">
         <v>28</v>
@@ -2628,10 +2628,10 @@
         <v>43.81649605606221</v>
       </c>
       <c r="D88" t="n">
-        <v>45.32141269841269</v>
+        <v>46.4848088023088</v>
       </c>
       <c r="E88" t="n">
-        <v>45.25927003249642</v>
+        <v>45.61929824988227</v>
       </c>
       <c r="F88" t="n">
         <v>28</v>
@@ -2653,10 +2653,10 @@
         <v>33.35085225249447</v>
       </c>
       <c r="D89" t="n">
-        <v>30.13829916488174</v>
+        <v>30.53688392534178</v>
       </c>
       <c r="E89" t="n">
-        <v>30.52560080784748</v>
+        <v>30.18736741972362</v>
       </c>
       <c r="F89" t="n">
         <v>27</v>
@@ -2678,10 +2678,10 @@
         <v>30.69755704308931</v>
       </c>
       <c r="D90" t="n">
-        <v>35.84513461466825</v>
+        <v>35.73262487104399</v>
       </c>
       <c r="E90" t="n">
-        <v>34.35955301360703</v>
+        <v>34.24849224216729</v>
       </c>
       <c r="F90" t="n">
         <v>27</v>
@@ -2703,10 +2703,10 @@
         <v>36.12961302917173</v>
       </c>
       <c r="D91" t="n">
-        <v>39.91971360509409</v>
+        <v>40.10060014882448</v>
       </c>
       <c r="E91" t="n">
-        <v>40.90947243026224</v>
+        <v>40.52417657427473</v>
       </c>
       <c r="F91" t="n">
         <v>27</v>
@@ -2728,10 +2728,10 @@
         <v>28.93093777562846</v>
       </c>
       <c r="D92" t="n">
-        <v>32.36851364950839</v>
+        <v>32.23481325472773</v>
       </c>
       <c r="E92" t="n">
-        <v>37.25992487944452</v>
+        <v>37.56887184018001</v>
       </c>
       <c r="F92" t="n">
         <v>27</v>
@@ -2753,10 +2753,10 @@
         <v>15.63816124042479</v>
       </c>
       <c r="D93" t="n">
-        <v>21.67</v>
+        <v>21.46</v>
       </c>
       <c r="E93" t="n">
-        <v>20.51330425265638</v>
+        <v>20.44020551999923</v>
       </c>
       <c r="F93" t="n">
         <v>27</v>
@@ -2778,10 +2778,10 @@
         <v>35.49084719664994</v>
       </c>
       <c r="D94" t="n">
-        <v>39.31493640193327</v>
+        <v>39.57038337058538</v>
       </c>
       <c r="E94" t="n">
-        <v>41.52836956645702</v>
+        <v>43.04960711620589</v>
       </c>
       <c r="F94" t="n">
         <v>27</v>
@@ -2803,10 +2803,10 @@
         <v>30.6253408453853</v>
       </c>
       <c r="D95" t="n">
-        <v>28.56523837567095</v>
+        <v>29.58910507255204</v>
       </c>
       <c r="E95" t="n">
-        <v>26.36171535565745</v>
+        <v>25.76319084581056</v>
       </c>
       <c r="F95" t="n">
         <v>27</v>
@@ -2828,10 +2828,10 @@
         <v>27.79850272091466</v>
       </c>
       <c r="D96" t="n">
-        <v>19.85</v>
+        <v>18.36020833333333</v>
       </c>
       <c r="E96" t="n">
-        <v>19.16336015686847</v>
+        <v>19.59268384118978</v>
       </c>
       <c r="F96" t="n">
         <v>27</v>
@@ -2853,10 +2853,10 @@
         <v>38.11582547637088</v>
       </c>
       <c r="D97" t="n">
-        <v>43.73840907628956</v>
+        <v>44.68911087115498</v>
       </c>
       <c r="E97" t="n">
-        <v>40.51248723428098</v>
+        <v>40.88128590831835</v>
       </c>
       <c r="F97" t="n">
         <v>27</v>
@@ -2878,10 +2878,10 @@
         <v>39.3287909382106</v>
       </c>
       <c r="D98" t="n">
-        <v>32.75017983535506</v>
+        <v>34.76313193931671</v>
       </c>
       <c r="E98" t="n">
-        <v>34.15954484488492</v>
+        <v>35.03150524947217</v>
       </c>
       <c r="F98" t="n">
         <v>27</v>
@@ -2903,10 +2903,10 @@
         <v>24.82971165125401</v>
       </c>
       <c r="D99" t="n">
-        <v>17.97384615384615</v>
+        <v>17.7393137254902</v>
       </c>
       <c r="E99" t="n">
-        <v>12.85178597175648</v>
+        <v>12.56756370423918</v>
       </c>
       <c r="F99" t="n">
         <v>27</v>
@@ -2928,10 +2928,10 @@
         <v>41.04860408715695</v>
       </c>
       <c r="D100" t="n">
-        <v>36.24671492970631</v>
+        <v>36.11489643281556</v>
       </c>
       <c r="E100" t="n">
-        <v>40.19435303257193</v>
+        <v>40.72414958089556</v>
       </c>
       <c r="F100" t="n">
         <v>27</v>
@@ -2953,10 +2953,10 @@
         <v>28.25809723096305</v>
       </c>
       <c r="D101" t="n">
-        <v>26.58</v>
+        <v>26.574</v>
       </c>
       <c r="E101" t="n">
-        <v>31.20992232049713</v>
+        <v>31.35266825141144</v>
       </c>
       <c r="F101" t="n">
         <v>27</v>

</xml_diff>